<commit_message>
Working on psychosocial queries, indexes on db, changing documentation file
</commit_message>
<xml_diff>
--- a/public/files/template-importacao-de-funcionarios-facilita.xlsx
+++ b/public/files/template-importacao-de-funcionarios-facilita.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Facilita_1\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42E46F35-4FC5-4F22-B738-A5DDD7B00F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A0887A-1B1D-4B07-8789-430B189F8F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F8D6858F-C36F-4EC2-8F8F-4FAC4690FCA0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Nome Completo</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Sexo do funcionario</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
 </sst>
 </file>
@@ -456,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78FD3D03-1648-4DD8-A169-4C41F5C3006D}">
   <dimension ref="A1:K274"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -505,7 +508,9 @@
       <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">

</xml_diff>